<commit_message>
time sheets GABY and attendance
</commit_message>
<xml_diff>
--- a/Admin/attendance-SPRING.xlsx
+++ b/Admin/attendance-SPRING.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SPONSOR" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">SPONSOR!$6:$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">TA!$A:$P</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">TA!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">TEAM!$A:$P</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">TEAM!$A:$S</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">TEAM!$6:$6</definedName>
     <definedName function="false" hidden="false" name="valuevx" vbProcedure="false">42.314159</definedName>
     <definedName function="false" hidden="false" name="vertex42_copyright" vbProcedure="false">"© 2017 Vertex42 LLC"</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="19">
   <si>
     <t xml:space="preserve">Sponsor Meetings</t>
   </si>
@@ -90,6 +90,9 @@
     <t xml:space="preserve">Feb </t>
   </si>
   <si>
+    <t xml:space="preserve">Apr</t>
+  </si>
+  <si>
     <t xml:space="preserve">TA Meetings</t>
   </si>
 </sst>
@@ -103,7 +106,7 @@
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -178,6 +181,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -324,7 +332,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,6 +430,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,8 +529,8 @@
   </sheetPr>
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5:F10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -602,8 +614,12 @@
       <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -638,8 +654,12 @@
       <c r="F4" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="H4" s="11" t="n">
+        <v>30</v>
+      </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -675,8 +695,12 @@
       <c r="F5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
@@ -685,7 +709,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
@@ -718,8 +742,12 @@
       <c r="F6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -728,7 +756,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="15" t="n">
         <f aca="false">COUNTA(C6:N6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P6" s="16" t="n">
         <f aca="false">O6/COUNTA($C$4:$N$4)</f>
@@ -761,8 +789,12 @@
       <c r="F7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -771,7 +803,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="15" t="n">
         <f aca="false">COUNTA(C7:N7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P7" s="16" t="n">
         <f aca="false">O7/COUNTA($C$4:$N$4)</f>
@@ -802,8 +834,12 @@
       <c r="F8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -812,7 +848,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="15" t="n">
         <f aca="false">COUNTA(C8:N8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P8" s="16" t="n">
         <f aca="false">O8/COUNTA($C$4:$N$4)</f>
@@ -839,8 +875,12 @@
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -849,11 +889,11 @@
       <c r="N9" s="14"/>
       <c r="O9" s="15" t="n">
         <f aca="false">COUNTA(C9:N9)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P9" s="16" t="n">
         <f aca="false">O9/COUNTA($C$4:$N$4)</f>
-        <v>0.5</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -880,8 +920,12 @@
       <c r="F10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -890,7 +934,7 @@
       <c r="N10" s="14"/>
       <c r="O10" s="15" t="n">
         <f aca="false">COUNTA(C10:N10)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P10" s="16" t="n">
         <f aca="false">O10/COUNTA($C$4:$N$4)</f>
@@ -948,11 +992,11 @@
       </c>
       <c r="G12" s="24" t="n">
         <f aca="false">COUNTA(G5:G11)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H12" s="24" t="n">
         <f aca="false">COUNTA(H5:H11)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I12" s="24" t="n">
         <f aca="false">COUNTA(I5:I11)</f>
@@ -1049,11 +1093,11 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:H10" type="list">
-      <formula1>checkbox</formula1>
+      <formula1>SPONSOR!checkbox</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I5:N10" type="list">
-      <formula1>checkbox</formula1>
+      <formula1>SPONSOR!checkbox</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1072,24 +1116,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="F5:F10 I9"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="1" width="4.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="4.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="10.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="1" width="4.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="4.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="21" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="10.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="24" style="1" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1111,12 +1155,15 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8"/>
@@ -1135,12 +1182,15 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
@@ -1168,23 +1218,40 @@
       <c r="I3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="9" t="s">
+      <c r="J3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
+      <c r="S3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="5"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
@@ -1210,19 +1277,36 @@
       <c r="I4" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
+      <c r="J4" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="K4" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="L4" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M4" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="N4" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="O4" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="P4" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="n">
@@ -1253,25 +1337,42 @@
       <c r="I5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="15" t="n">
-        <f aca="false">COUNTA(C5:N5)</f>
-        <v>7</v>
-      </c>
-      <c r="P5" s="16" t="n">
-        <f aca="false">O5/COUNTA($C$4:$N$4)</f>
+      <c r="J5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="15" t="n">
+        <f aca="false">COUNTA(C5:P5)</f>
+        <v>14</v>
+      </c>
+      <c r="S5" s="16" t="n">
+        <f aca="false">R5/COUNTA($C$4:$P$4)</f>
         <v>1</v>
       </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="n">
@@ -1302,25 +1403,42 @@
       <c r="I6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="15" t="n">
-        <f aca="false">COUNTA(C6:N6)</f>
-        <v>7</v>
-      </c>
-      <c r="P6" s="16" t="n">
-        <f aca="false">O6/COUNTA($C$4:$N$4)</f>
+      <c r="J6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="15" t="n">
+        <f aca="false">COUNTA(C6:P6)</f>
+        <v>14</v>
+      </c>
+      <c r="S6" s="16" t="n">
+        <f aca="false">R6/COUNTA($C$4:$P$4)</f>
         <v>1</v>
       </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
     </row>
     <row r="7" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="n">
@@ -1351,23 +1469,40 @@
       <c r="I7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="15" t="n">
-        <f aca="false">COUNTA(C7:N7)</f>
-        <v>7</v>
-      </c>
-      <c r="P7" s="16" t="n">
-        <f aca="false">O7/COUNTA($C$4:$N$4)</f>
+      <c r="J7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="15" t="n">
+        <f aca="false">COUNTA(C7:P7)</f>
+        <v>14</v>
+      </c>
+      <c r="S7" s="16" t="n">
+        <f aca="false">R7/COUNTA($C$4:$P$4)</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
     </row>
     <row r="8" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="n">
@@ -1398,23 +1533,40 @@
       <c r="I8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="15" t="n">
-        <f aca="false">COUNTA(C8:N8)</f>
-        <v>7</v>
-      </c>
-      <c r="P8" s="16" t="n">
-        <f aca="false">O8/COUNTA($C$4:$N$4)</f>
+      <c r="J8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="15" t="n">
+        <f aca="false">COUNTA(C8:P8)</f>
+        <v>14</v>
+      </c>
+      <c r="S8" s="16" t="n">
+        <f aca="false">R8/COUNTA($C$4:$P$4)</f>
         <v>1</v>
       </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
     </row>
     <row r="9" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="n">
@@ -1441,23 +1593,32 @@
       <c r="I9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="J9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="15" t="n">
-        <f aca="false">COUNTA(C9:N9)</f>
-        <v>5</v>
-      </c>
-      <c r="P9" s="16" t="n">
-        <f aca="false">O9/COUNTA($C$4:$N$4)</f>
-        <v>0.714285714285714</v>
-      </c>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="15" t="n">
+        <f aca="false">COUNTA(C9:P9)</f>
+        <v>8</v>
+      </c>
+      <c r="S9" s="16" t="n">
+        <f aca="false">R9/COUNTA($C$4:$P$4)</f>
+        <v>0.571428571428571</v>
+      </c>
       <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
     </row>
     <row r="10" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="n">
@@ -1488,23 +1649,40 @@
       <c r="I10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="15" t="n">
-        <f aca="false">COUNTA(C10:N10)</f>
-        <v>7</v>
-      </c>
-      <c r="P10" s="16" t="n">
-        <f aca="false">O10/COUNTA($C$4:$N$4)</f>
+      <c r="J10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="15" t="n">
+        <f aca="false">COUNTA(C10:P10)</f>
+        <v>14</v>
+      </c>
+      <c r="S10" s="16" t="n">
+        <f aca="false">R10/COUNTA($C$4:$P$4)</f>
         <v>1</v>
       </c>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
     </row>
     <row r="11" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17"/>
@@ -1521,14 +1699,17 @@
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
       <c r="T11" s="2"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
     </row>
     <row r="12" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22"/>
@@ -1565,29 +1746,41 @@
       </c>
       <c r="J12" s="24" t="n">
         <f aca="false">COUNTA(J5:J11)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K12" s="24" t="n">
         <f aca="false">COUNTA(K5:K11)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="24"/>
+        <v>6</v>
+      </c>
+      <c r="L12" s="25" t="n">
+        <f aca="false">COUNTA(L5:L11)</f>
+        <v>6</v>
+      </c>
       <c r="M12" s="24" t="n">
         <f aca="false">COUNTA(M5:M11)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N12" s="24" t="n">
-        <f aca="false">COUNTA(N5:N11)</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+        <f aca="false">COUNTA(N5:N10)</f>
+        <v>5</v>
+      </c>
+      <c r="O12" s="24" t="n">
+        <f aca="false">COUNTA(O5:O11)</f>
+        <v>5</v>
+      </c>
+      <c r="P12" s="24" t="n">
+        <f aca="false">COUNTA(P5:P11)</f>
+        <v>5</v>
+      </c>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
       <c r="T12" s="2"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
     </row>
     <row r="13" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
@@ -1606,12 +1799,15 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
       <c r="T13" s="2"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
     </row>
     <row r="14" s="7" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
@@ -1630,30 +1826,37 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
       <c r="T14" s="2"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:B4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C3:N3" type="list">
+  <dataValidations count="5">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C3:Q3" type="list">
       <formula1>"Jan,Feb,Mar,Apr,May,Jun,Jul,Aug,Sep,Oct,Nov,Dec"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C4:N4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C4:Q4" type="list">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J5:N10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J5:P10" type="list">
+      <formula1>TEAM!checkbox</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q5:Q10" type="list">
       <formula1>TEAM!checkbox</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1680,13 +1883,13 @@
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="F5:F10 D9"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="26.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="26.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="1" width="4.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="4.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7"/>
@@ -1699,7 +1902,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="2"/>
@@ -1725,7 +1928,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8"/>
-      <c r="B2" s="26"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1758,8 +1961,12 @@
       <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -1790,8 +1997,12 @@
       <c r="D4" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>6</v>
+      </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -1823,8 +2034,12 @@
       <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1835,7 +2050,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
@@ -1862,8 +2077,12 @@
       <c r="D6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1874,7 +2093,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="15" t="n">
         <f aca="false">COUNTA(C6:N6)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P6" s="16" t="n">
         <f aca="false">O6/COUNTA($C$4:$N$4)</f>
@@ -1901,8 +2120,12 @@
       <c r="D7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -1913,7 +2136,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="15" t="n">
         <f aca="false">COUNTA(C7:N7)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P7" s="16" t="n">
         <f aca="false">O7/COUNTA($C$4:$N$4)</f>
@@ -1938,8 +2161,12 @@
       <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -1950,7 +2177,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="15" t="n">
         <f aca="false">COUNTA(C8:N8)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P8" s="16" t="n">
         <f aca="false">O8/COUNTA($C$4:$N$4)</f>
@@ -1973,7 +2200,9 @@
       <c r="D9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1985,7 +2214,7 @@
       <c r="N9" s="14"/>
       <c r="O9" s="15" t="n">
         <f aca="false">COUNTA(C9:N9)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="16" t="n">
         <f aca="false">O9/COUNTA($C$4:$N$4)</f>
@@ -2010,8 +2239,12 @@
       <c r="D10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2022,7 +2255,7 @@
       <c r="N10" s="14"/>
       <c r="O10" s="15" t="n">
         <f aca="false">COUNTA(C10:N10)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P10" s="16" t="n">
         <f aca="false">O10/COUNTA($C$4:$N$4)</f>
@@ -2035,7 +2268,7 @@
     </row>
     <row r="11" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17"/>
-      <c r="B11" s="27"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -2072,11 +2305,11 @@
       </c>
       <c r="E12" s="24" t="n">
         <f aca="false">COUNTA(E5:E11)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F12" s="24" t="n">
         <f aca="false">COUNTA(F5:F11)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G12" s="24" t="n">
         <f aca="false">COUNTA(G5:G11)</f>
@@ -2118,7 +2351,7 @@
     </row>
     <row r="13" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
-      <c r="B13" s="25"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2142,7 +2375,7 @@
     </row>
     <row r="14" s="7" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
-      <c r="B14" s="25"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2180,11 +2413,11 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E5:N10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G5:N10" type="list">
       <formula1>TEAM!checkbox</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:D10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:F10" type="list">
       <formula1>checkbox</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>